<commit_message>
D. J.: - Added a command to display tabular permissions overview (#21) - Simplified help command - Added a command to display the ids of the roles/text channels to better work with !role and !text_channel - Removed voice_channel for simplicity - Updated the default configuration - Updated the UC file
</commit_message>
<xml_diff>
--- a/UC-DB.xlsx
+++ b/UC-DB.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis\projects\discord-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C64D6A-82A4-409F-8595-5212F0082FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526AED22-10DF-4ED2-869F-08374BC23166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Use Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="UC1" sheetId="2" r:id="rId1"/>
+    <sheet name="UC2" sheetId="3" r:id="rId2"/>
+    <sheet name="UC3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="57">
   <si>
     <t>Umfeld</t>
   </si>
@@ -164,9 +166,6 @@
   </si>
   <si>
     <t>Nutzer schreibt im Text-Channel "!reset"</t>
-  </si>
-  <si>
-    <t>Nutzer schreibt im Text-Channel "!volume 10"</t>
   </si>
   <si>
     <t>Musikbot anfordern und steuern</t>
@@ -200,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,21 +227,6 @@
       <b/>
       <sz val="16"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,24 +327,21 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,45 +649,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I120"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7648C3-7EE1-44A5-A67E-62E5B872AD10}">
+  <dimension ref="B1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -722,8 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -731,21 +703,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -753,19 +720,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -773,13 +735,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -787,21 +749,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -809,11 +766,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <v>1</v>
       </c>
       <c r="D16" t="s">
@@ -822,7 +779,7 @@
     </row>
     <row r="17" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>2</v>
       </c>
       <c r="D17" t="s">
@@ -831,7 +788,7 @@
     </row>
     <row r="18" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>3</v>
       </c>
       <c r="D18" t="s">
@@ -840,7 +797,7 @@
     </row>
     <row r="19" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="11">
+      <c r="C19" s="8">
         <v>4</v>
       </c>
       <c r="D19" t="s">
@@ -849,7 +806,7 @@
     </row>
     <row r="20" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>5</v>
       </c>
       <c r="D20" t="s">
@@ -858,7 +815,7 @@
     </row>
     <row r="21" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="11">
+      <c r="C21" s="8">
         <v>6</v>
       </c>
       <c r="D21" t="s">
@@ -867,7 +824,7 @@
     </row>
     <row r="22" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="10">
+      <c r="C22" s="7">
         <v>7</v>
       </c>
       <c r="D22" t="s">
@@ -876,7 +833,7 @@
     </row>
     <row r="23" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="11">
+      <c r="C23" s="8">
         <v>8</v>
       </c>
       <c r="D23" t="s">
@@ -885,7 +842,7 @@
     </row>
     <row r="24" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <v>7</v>
       </c>
       <c r="D24" t="s">
@@ -894,7 +851,7 @@
     </row>
     <row r="25" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="11">
+      <c r="C25" s="8">
         <v>8</v>
       </c>
       <c r="D25" t="s">
@@ -903,7 +860,7 @@
     </row>
     <row r="26" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
-      <c r="C26" s="10">
+      <c r="C26" s="7">
         <v>9</v>
       </c>
       <c r="D26" t="s">
@@ -912,7 +869,7 @@
     </row>
     <row r="27" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
-      <c r="C27" s="11">
+      <c r="C27" s="8">
         <v>10</v>
       </c>
       <c r="D27" t="s">
@@ -921,7 +878,7 @@
     </row>
     <row r="28" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
-      <c r="C28" s="10">
+      <c r="C28" s="7">
         <v>11</v>
       </c>
       <c r="D28" t="s">
@@ -930,7 +887,7 @@
     </row>
     <row r="29" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
-      <c r="C29" s="11">
+      <c r="C29" s="8">
         <v>12</v>
       </c>
       <c r="D29" t="s">
@@ -939,7 +896,7 @@
     </row>
     <row r="30" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
-      <c r="C30" s="10">
+      <c r="C30" s="7">
         <v>13</v>
       </c>
       <c r="D30" t="s">
@@ -948,7 +905,7 @@
     </row>
     <row r="31" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
-      <c r="C31" s="11">
+      <c r="C31" s="8">
         <v>14</v>
       </c>
       <c r="D31" t="s">
@@ -957,7 +914,7 @@
     </row>
     <row r="32" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
-      <c r="C32" s="10">
+      <c r="C32" s="7">
         <v>15</v>
       </c>
       <c r="D32" t="s">
@@ -966,7 +923,7 @@
     </row>
     <row r="33" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
-      <c r="C33" s="11">
+      <c r="C33" s="8">
         <v>16</v>
       </c>
       <c r="D33" t="s">
@@ -975,7 +932,7 @@
     </row>
     <row r="34" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
-      <c r="C34" s="10">
+      <c r="C34" s="7">
         <v>17</v>
       </c>
       <c r="D34" t="s">
@@ -984,7 +941,7 @@
     </row>
     <row r="35" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
-      <c r="C35" s="11">
+      <c r="C35" s="8">
         <v>18</v>
       </c>
       <c r="D35" t="s">
@@ -993,7 +950,7 @@
     </row>
     <row r="36" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
-      <c r="C36" s="10">
+      <c r="C36" s="7">
         <v>19</v>
       </c>
       <c r="D36" t="s">
@@ -1002,7 +959,7 @@
     </row>
     <row r="37" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
-      <c r="C37" s="11">
+      <c r="C37" s="8">
         <v>20</v>
       </c>
       <c r="D37" t="s">
@@ -1011,7 +968,7 @@
     </row>
     <row r="38" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
-      <c r="C38" s="10">
+      <c r="C38" s="7">
         <v>21</v>
       </c>
       <c r="D38" t="s">
@@ -1020,7 +977,7 @@
     </row>
     <row r="39" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
-      <c r="C39" s="11">
+      <c r="C39" s="8">
         <v>22</v>
       </c>
       <c r="D39" t="s">
@@ -1029,7 +986,7 @@
     </row>
     <row r="40" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
-      <c r="C40" s="10">
+      <c r="C40" s="7">
         <v>23</v>
       </c>
       <c r="D40" t="s">
@@ -1038,7 +995,7 @@
     </row>
     <row r="41" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
-      <c r="C41" s="11">
+      <c r="C41" s="8">
         <v>24</v>
       </c>
       <c r="D41" t="s">
@@ -1047,7 +1004,7 @@
     </row>
     <row r="42" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
-      <c r="C42" s="10">
+      <c r="C42" s="7">
         <v>25</v>
       </c>
       <c r="D42" t="s">
@@ -1056,7 +1013,7 @@
     </row>
     <row r="43" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
-      <c r="C43" s="11">
+      <c r="C43" s="8">
         <v>26</v>
       </c>
       <c r="D43" t="s">
@@ -1065,7 +1022,7 @@
     </row>
     <row r="44" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
-      <c r="C44" s="10">
+      <c r="C44" s="7">
         <v>27</v>
       </c>
       <c r="D44" t="s">
@@ -1074,7 +1031,7 @@
     </row>
     <row r="45" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
-      <c r="C45" s="11">
+      <c r="C45" s="8">
         <v>28</v>
       </c>
       <c r="D45" t="s">
@@ -1082,620 +1039,649 @@
       </c>
     </row>
     <row r="46" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="8" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1519DEC2-0321-4208-8F3C-21256601B2C7}">
+  <dimension ref="B1:F38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="8">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="7">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="8">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="7">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="8">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="7">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="8">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="7">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="8">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="7">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="8">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="7">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="8">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="7">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="8">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="7">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="8">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="7">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="8">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="7">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="8">
+        <v>22</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155F45C3-FD08-4830-9F41-11DE356FAAE1}">
+  <dimension ref="B1:D38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C57" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
+      <c r="C13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
+      <c r="C14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="1" t="s">
+    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C16" s="7">
         <v>1</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="1"/>
-      <c r="C61" s="11">
+    <row r="17" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="8">
         <v>2</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="1"/>
-      <c r="C62" s="10">
+    <row r="18" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="7">
         <v>3</v>
       </c>
-      <c r="D62" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="1"/>
-      <c r="C63" s="11">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="8">
         <v>4</v>
       </c>
-      <c r="D63" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="1"/>
-      <c r="C64" s="10">
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="C20" s="7">
         <v>5</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="8">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="7">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="8">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="7">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="8">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="7">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="8">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+      <c r="C28" s="7">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="8">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+      <c r="C30" s="7">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+      <c r="C31" s="8">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+      <c r="C32" s="7">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="8">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+      <c r="C34" s="7">
+        <v>19</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="8">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="7">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="1"/>
-      <c r="C65" s="11">
-        <v>6</v>
-      </c>
-      <c r="D65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="1"/>
-      <c r="C66" s="10">
-        <v>7</v>
-      </c>
-      <c r="D66" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="1"/>
-      <c r="C67" s="11">
-        <v>8</v>
-      </c>
-      <c r="D67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="1"/>
-      <c r="C68" s="10">
-        <v>9</v>
-      </c>
-      <c r="D68" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="1"/>
-      <c r="C69" s="11">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="1"/>
-      <c r="C70" s="10">
-        <v>11</v>
-      </c>
-      <c r="D70" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="1"/>
-      <c r="C71" s="11">
-        <v>12</v>
-      </c>
-      <c r="D71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="1"/>
-      <c r="C72" s="10">
-        <v>13</v>
-      </c>
-      <c r="D72" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="1"/>
-      <c r="C73" s="11">
-        <v>14</v>
-      </c>
-      <c r="D73" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="1"/>
-      <c r="C74" s="10">
-        <v>15</v>
-      </c>
-      <c r="D74" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="1"/>
-      <c r="C75" s="11">
-        <v>16</v>
-      </c>
-      <c r="D75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="1"/>
-      <c r="C76" s="10">
-        <v>17</v>
-      </c>
-      <c r="D76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="1"/>
-      <c r="C77" s="11">
-        <v>18</v>
-      </c>
-      <c r="D77" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="1"/>
-      <c r="C78" s="10">
-        <v>19</v>
-      </c>
-      <c r="D78" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="1"/>
-      <c r="C79" s="11">
-        <v>20</v>
-      </c>
-      <c r="D79" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="1"/>
-      <c r="C80" s="10">
-        <v>21</v>
-      </c>
-      <c r="D80" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="1"/>
-      <c r="C81" s="11">
+    <row r="37" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="8">
         <v>22</v>
       </c>
-      <c r="D81" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="1"/>
-      <c r="C82" s="10">
-        <v>25</v>
-      </c>
-      <c r="D82" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="1"/>
-      <c r="C83" s="11">
-        <v>26</v>
-      </c>
-      <c r="D83" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D86" s="8"/>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C87" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C89" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D90" s="9"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C93" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="1"/>
-      <c r="C94" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D96" s="9"/>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C97" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C98" s="10">
-        <v>1</v>
-      </c>
-      <c r="D98" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="1"/>
-      <c r="C99" s="11">
-        <v>2</v>
-      </c>
-      <c r="D99" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="1"/>
-      <c r="C100" s="10">
-        <v>3</v>
-      </c>
-      <c r="D100" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="1"/>
-      <c r="C101" s="11">
-        <v>4</v>
-      </c>
-      <c r="D101" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="1"/>
-      <c r="C102" s="10">
-        <v>5</v>
-      </c>
-      <c r="D102" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="1"/>
-      <c r="C103" s="11">
-        <v>6</v>
-      </c>
-      <c r="D103" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="1"/>
-      <c r="C104" s="10">
-        <v>7</v>
-      </c>
-      <c r="D104" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="1"/>
-      <c r="C105" s="11">
-        <v>8</v>
-      </c>
-      <c r="D105" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="106" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="1"/>
-      <c r="C106" s="10">
-        <v>9</v>
-      </c>
-      <c r="D106" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="1"/>
-      <c r="C107" s="11">
-        <v>10</v>
-      </c>
-      <c r="D107" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="1"/>
-      <c r="C108" s="10">
-        <v>11</v>
-      </c>
-      <c r="D108" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="1"/>
-      <c r="C109" s="11">
-        <v>12</v>
-      </c>
-      <c r="D109" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="1"/>
-      <c r="C110" s="10">
-        <v>13</v>
-      </c>
-      <c r="D110" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="1"/>
-      <c r="C111" s="11">
-        <v>14</v>
-      </c>
-      <c r="D111" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="1"/>
-      <c r="C112" s="10">
-        <v>15</v>
-      </c>
-      <c r="D112" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="1"/>
-      <c r="C113" s="11">
-        <v>16</v>
-      </c>
-      <c r="D113" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="1"/>
-      <c r="C114" s="10">
-        <v>17</v>
-      </c>
-      <c r="D114" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="1"/>
-      <c r="C115" s="11">
-        <v>18</v>
-      </c>
-      <c r="D115" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="1"/>
-      <c r="C116" s="10">
-        <v>19</v>
-      </c>
-      <c r="D116" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="117" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="1"/>
-      <c r="C117" s="11">
-        <v>20</v>
-      </c>
-      <c r="D117" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="1"/>
-      <c r="C118" s="10">
-        <v>21</v>
-      </c>
-      <c r="D118" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="1"/>
-      <c r="C119" s="11">
-        <v>22</v>
-      </c>
-      <c r="D119" t="s">
+      <c r="D37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>